<commit_message>
Réorganisation du projet en dossiers famous_faceV1 et matching_unknown_faceV1
</commit_message>
<xml_diff>
--- a/resultats_test.xlsx
+++ b/resultats_test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,11 +545,7 @@
           <t>click</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
         <v>31</v>
       </c>
@@ -560,6 +556,782 @@
       </c>
       <c r="I3" t="n">
         <v>0.219</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>f544c96a-6197-4d0d-b592-8fcb3457baff</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>cv c</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-05-16 14:58:50</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>[5.514]</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>5.514</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>f698ae52-0426-42f1-b1a8-573953ae1ff5</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>cv v</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2025-05-16 22:54:20</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>[3.835]</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>3.835</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>be2ed463-ac60-4506-850e-fe200006ae81</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>cv v</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2025-05-16 22:54:40</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>[6.362]</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>6.362</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>7841f625-478d-4166-a398-9d3922c49b66</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>cv v</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025-05-16 23:02:48</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>[114.984]</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>114.984</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>9297f90f-f40a-4da3-90a4-97f05af87f95</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>cv c</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2025-05-16 23:09:11</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>9b76e222-a8c7-40cf-a62c-b65891f64a41</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>cv c</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-05-16 23:09:13</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>72c83084-1422-4a5a-aed3-7dd398d7d844</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>cv c</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-05-16 23:09:19</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>3be6b214-cf11-4cb9-9304-301319ec7253</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>c c</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2025-05-16 23:22:47</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="n">
+        <v>3</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>[3.546, 1.433, 1.051, 1.782, 2.082, 1.405, 1.606, 1.444, 1.015, 1.007, 0.929, 0.906, 1.507, 1.797, 0.969, 1.537, 3.081, 1.641, 1.94, 1.389, 1.421, 1.217, 0.95, 1.932, 1.732, 1.232, 1.557, 1.952, 1.215, 1.238, 1.192, 0.922, 2.218, 3.734, 1.538, 1.094, 1.183, 1.628, 1.521, 1.069, 1.136, 1.704, 2.718, 2.119, 1.208, 1.186, 2.094, 1.246, 0.957]</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>1.571</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>a986f675-2308-49a0-88a2-63275daa88ca</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>g g</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2025-05-16 23:44:28</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="n">
+        <v>26</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>[1.872, 2.413, 1.296, 0.966, 1.46, 2.015, 1.645, 1.162, 0.968, 1.207, 0.479, 0.866, 0.388, 0.858, 0.383, 0.368, 0.358, 0.377, 0.369, 0.394, 0.388, 0.479, 0.576, 0.344, 0.347, 0.313, 0.334, 0.379, 0.369, 0.361, 0.346, 0.35, 0.327, 0.357, 0.376, 0.413, 0.386, 0.429, 0.384, 0.321, 0.363, 0.314, 0.327, 0.406, 0.355, 0.379, 0.326, 0.273, 0.362]</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>0.623</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>e8d34b7a-eac8-40ff-bab1-50411e96fb1c</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>b b</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2025-05-16 23:54:19</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>33</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>[10.567, 3.331, 2.101, 2.908, 1.444, 1.572, 1.315, 0.266, 0.202, 0.171, 0.166, 0.163, 0.144, 0.144, 0.145, 0.117, 0.172, 0.081, 0.159, 0.106, 0.157, 0.053, 0.123, 0.042, 0.098, 0.077, 0.094, 0.045, 0.118, 0.06, 0.134, 0.064, 0.118, 0.101, 0.145, 0.075, 0.187, 0.163, 0.171, 0.199, 0.159, 0.122, 0.097, 0.145, 0.236, 0.141, 0.129, 0.142, 0.154]</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>0.588</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>0e624559-7627-4819-8b31-bd3f34eca3c7</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>c v</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2025-05-17 14:53:16</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>[35.15, 1.321, 0.843]</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>12.438</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>b417026a-e910-4230-8ba5-d4d95eb543c6</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>c v</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2025-05-17 14:57:12</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>space</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>[5.197, 3.134]</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>4.165</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>d9bded9f-a2dc-4762-b0cf-e19e06b1423d</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>c v</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2025-05-17 14:58:25</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>timer</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" t="n">
+        <v>20</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>[2, 2, 2, 0.927, 1.283, 1.635, 0.695, 1.079, 0.932, 0.775, 0.701, 0.882, 0.768, 1.151, 1.452, 1.063, 0.858, 0.69, 0.635, 0.664, 0.479, 0.277, 0.271, 0.579, 0.741, 0.599, 1.339, 0.95, 1.284, 0.598, 1.274, 1.291, 1.118, 0.728, 0.785, 1.091, 0.491, 0.347, 0.267, 0.226, 0.225, 0.249, 0.224, 0.212, 0.243, 0.26, 0.269, 0.255, 0.229]</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>0.798</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>cd3e81ab-ff2e-4b16-847a-99a517c91f91</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>gg y</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2025-05-17 23:16:54</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>space</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>[14.396, 0.987, 1.96, 2.636, 1.042, 0.595, 0.62, 2.127]</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>3.045</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>4ae26bd9-a061-4dd5-9bd6-ba565d9975ef</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>cc b</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2025-05-20 14:40:30</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>[10.448, 2.567, 0.912, 0.941]</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>3.717</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>28f3c421-a869-4952-b6b9-6b7bb826aa3c</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>cc b</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2025-05-20 14:47:02</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>44c59b08-5417-455b-84f5-77283c987fcd</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>g k</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2025-05-20 15:15:03</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="n">
+        <v>5</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>[14.396, 1.453, 1.271, 2.521, 3.04, 10.15, 1.917, 1.928, 1.257, 3.376, 1.121, 1.016, 0.777]</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>3.402</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>a15d14e0-60a5-4f69-afa1-1603f6af0cb3</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>gg k</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2025-05-20 15:38:02</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>[3.901, 13.457, 1.386, 3.122, 1.648, 1.947, 1.714, 0.847, 1.164, 6.089, 2.128, 2.212]</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>3.301</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>546594cd-3a96-406c-8d26-109094624088</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>gg k</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2025-05-20 15:38:19</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>6a5b97ed-9b98-4e90-a06d-76cebb8557ed</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>bb h</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-05-20 15:47:23</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>famous_face</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>2</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>[4.8, 1.832, 1.898, 1.793, 2.087, 1.641]</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>2.342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>